<commit_message>
Republish with added conditions.
</commit_message>
<xml_diff>
--- a/docs/CareConnect-BloodPressure-Observation-1.xlsx
+++ b/docs/CareConnect-BloodPressure-Observation-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10429" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10429" uniqueCount="716">
   <si>
     <t>Path</t>
   </si>
@@ -1565,7 +1565,7 @@
     <t>A code from the SNOMED Clinical Terminology UK with the expression (&lt;&lt;442083009 |anatomical or acquired body structure|).</t>
   </si>
   <si>
-    <t xml:space="preserve">https://fhir.hl7.org.uk/STU3/ValueSet/CareConnect-BodySite-1 </t>
+    <t>https://fhir.hl7.org.uk/STU3/ValueSet/CareConnect-BodySite-1</t>
   </si>
   <si>
     <t>Observation.bodySite.coding.id</t>
@@ -2105,7 +2105,7 @@
     <t>Component results</t>
   </si>
   <si>
-    <t xml:space="preserve">http://hl7.org/fhir/stu3/valueset-observation-vitalsignresult.html </t>
+    <t>http://hl7.org/fhir/stu3/valueset-observation-vitalsignresult.html</t>
   </si>
   <si>
     <t>Observation.component.code.id</t>
@@ -2118,9 +2118,6 @@
   </si>
   <si>
     <t>Systolic Blood Pressure</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/stu3/valueset-observation-vitalsignresult.html</t>
   </si>
   <si>
     <t>Observation.component.code.coding.id</t>
@@ -24409,7 +24406,7 @@
         <v>291</v>
       </c>
       <c r="Y188" t="s" s="2">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="Z188" t="s" s="2">
         <v>45</v>
@@ -24462,7 +24459,7 @@
     </row>
     <row r="189" hidden="true">
       <c r="A189" t="s" s="2">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B189" s="2"/>
       <c r="C189" t="s" s="2">
@@ -24577,7 +24574,7 @@
     </row>
     <row r="190" hidden="true">
       <c r="A190" t="s" s="2">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B190" s="2"/>
       <c r="C190" t="s" s="2">
@@ -24694,7 +24691,7 @@
     </row>
     <row r="191" hidden="true">
       <c r="A191" t="s" s="2">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B191" s="2"/>
       <c r="C191" t="s" s="2">
@@ -24813,7 +24810,7 @@
     </row>
     <row r="192" hidden="true">
       <c r="A192" t="s" s="2">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" t="s" s="2">
@@ -24930,7 +24927,7 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B193" s="2"/>
       <c r="C193" t="s" s="2">
@@ -24970,7 +24967,7 @@
       </c>
       <c r="P193" s="2"/>
       <c r="Q193" t="s" s="2">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="R193" t="s" s="2">
         <v>45</v>
@@ -25047,7 +25044,7 @@
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B194" s="2"/>
       <c r="C194" t="s" s="2">
@@ -25164,7 +25161,7 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" t="s" s="2">
@@ -25404,7 +25401,7 @@
     </row>
     <row r="197" hidden="true">
       <c r="A197" t="s" s="2">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B197" s="2"/>
       <c r="C197" t="s" s="2">
@@ -25519,7 +25516,7 @@
     </row>
     <row r="198" hidden="true">
       <c r="A198" t="s" s="2">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" t="s" s="2">
@@ -25634,7 +25631,7 @@
     </row>
     <row r="199" hidden="true">
       <c r="A199" t="s" s="2">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B199" t="s" s="2">
         <v>304</v>
@@ -25751,7 +25748,7 @@
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B200" s="2"/>
       <c r="C200" t="s" s="2">
@@ -25866,7 +25863,7 @@
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B201" s="2"/>
       <c r="C201" t="s" s="2">
@@ -25981,7 +25978,7 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B202" t="s" s="2">
         <v>310</v>
@@ -26098,7 +26095,7 @@
     </row>
     <row r="203" hidden="true">
       <c r="A203" t="s" s="2">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B203" s="2"/>
       <c r="C203" t="s" s="2">
@@ -26213,7 +26210,7 @@
     </row>
     <row r="204" hidden="true">
       <c r="A204" t="s" s="2">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B204" s="2"/>
       <c r="C204" t="s" s="2">
@@ -26330,7 +26327,7 @@
     </row>
     <row r="205" hidden="true">
       <c r="A205" t="s" s="2">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B205" s="2"/>
       <c r="C205" t="s" s="2">
@@ -26447,7 +26444,7 @@
     </row>
     <row r="206" hidden="true">
       <c r="A206" t="s" s="2">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B206" t="s" s="2">
         <v>320</v>
@@ -26564,7 +26561,7 @@
     </row>
     <row r="207" hidden="true">
       <c r="A207" t="s" s="2">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B207" t="s" s="2">
         <v>323</v>
@@ -26681,7 +26678,7 @@
     </row>
     <row r="208" hidden="true">
       <c r="A208" t="s" s="2">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B208" s="2"/>
       <c r="C208" t="s" s="2">
@@ -26796,7 +26793,7 @@
     </row>
     <row r="209" hidden="true">
       <c r="A209" t="s" s="2">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B209" s="2"/>
       <c r="C209" t="s" s="2">
@@ -26913,7 +26910,7 @@
     </row>
     <row r="210" hidden="true">
       <c r="A210" t="s" s="2">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B210" s="2"/>
       <c r="C210" t="s" s="2">
@@ -27030,7 +27027,7 @@
     </row>
     <row r="211" hidden="true">
       <c r="A211" t="s" s="2">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B211" t="s" s="2">
         <v>326</v>
@@ -27147,7 +27144,7 @@
     </row>
     <row r="212" hidden="true">
       <c r="A212" t="s" s="2">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B212" s="2"/>
       <c r="C212" t="s" s="2">
@@ -27264,7 +27261,7 @@
     </row>
     <row r="213" hidden="true">
       <c r="A213" t="s" s="2">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B213" s="2"/>
       <c r="C213" t="s" s="2">
@@ -27379,7 +27376,7 @@
     </row>
     <row r="214" hidden="true">
       <c r="A214" t="s" s="2">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B214" s="2"/>
       <c r="C214" t="s" s="2">
@@ -27498,7 +27495,7 @@
     </row>
     <row r="215" hidden="true">
       <c r="A215" t="s" s="2">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B215" s="2"/>
       <c r="C215" t="s" s="2">
@@ -27615,7 +27612,7 @@
     </row>
     <row r="216" hidden="true">
       <c r="A216" t="s" s="2">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B216" s="2"/>
       <c r="C216" t="s" s="2">
@@ -27655,7 +27652,7 @@
       </c>
       <c r="P216" s="2"/>
       <c r="Q216" t="s" s="2">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="R216" t="s" s="2">
         <v>45</v>
@@ -27732,7 +27729,7 @@
     </row>
     <row r="217" hidden="true">
       <c r="A217" t="s" s="2">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B217" s="2"/>
       <c r="C217" t="s" s="2">
@@ -27772,7 +27769,7 @@
       </c>
       <c r="P217" s="2"/>
       <c r="Q217" t="s" s="2">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="R217" t="s" s="2">
         <v>45</v>
@@ -27849,7 +27846,7 @@
     </row>
     <row r="218" hidden="true">
       <c r="A218" t="s" s="2">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B218" s="2"/>
       <c r="C218" t="s" s="2">
@@ -27968,7 +27965,7 @@
     </row>
     <row r="219" hidden="true">
       <c r="A219" t="s" s="2">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B219" s="2"/>
       <c r="C219" t="s" s="2">
@@ -28087,7 +28084,7 @@
     </row>
     <row r="220" hidden="true">
       <c r="A220" t="s" s="2">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B220" t="s" s="2">
         <v>386</v>
@@ -28152,10 +28149,10 @@
         <v>136</v>
       </c>
       <c r="X220" t="s" s="2">
+        <v>700</v>
+      </c>
+      <c r="Y220" t="s" s="2">
         <v>701</v>
-      </c>
-      <c r="Y220" t="s" s="2">
-        <v>702</v>
       </c>
       <c r="Z220" t="s" s="2">
         <v>45</v>
@@ -28208,7 +28205,7 @@
     </row>
     <row r="221" hidden="true">
       <c r="A221" t="s" s="2">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B221" s="2"/>
       <c r="C221" t="s" s="2">
@@ -28323,7 +28320,7 @@
     </row>
     <row r="222" hidden="true">
       <c r="A222" t="s" s="2">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B222" s="2"/>
       <c r="C222" t="s" s="2">
@@ -28440,7 +28437,7 @@
     </row>
     <row r="223" hidden="true">
       <c r="A223" t="s" s="2">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B223" s="2"/>
       <c r="C223" t="s" s="2">
@@ -28559,7 +28556,7 @@
     </row>
     <row r="224" hidden="true">
       <c r="A224" t="s" s="2">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B224" s="2"/>
       <c r="C224" t="s" s="2">
@@ -28680,7 +28677,7 @@
     </row>
     <row r="225" hidden="true">
       <c r="A225" t="s" s="2">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B225" s="2"/>
       <c r="C225" t="s" s="2">
@@ -28797,7 +28794,7 @@
     </row>
     <row r="226" hidden="true">
       <c r="A226" t="s" s="2">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B226" s="2"/>
       <c r="C226" t="s" s="2">
@@ -28914,7 +28911,7 @@
     </row>
     <row r="227" hidden="true">
       <c r="A227" t="s" s="2">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B227" s="2"/>
       <c r="C227" t="s" s="2">
@@ -28940,7 +28937,7 @@
         <v>75</v>
       </c>
       <c r="K227" t="s" s="2">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="L227" t="s" s="2">
         <v>438</v>
@@ -28956,7 +28953,7 @@
       </c>
       <c r="P227" s="2"/>
       <c r="Q227" t="s" s="2">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="R227" t="s" s="2">
         <v>45</v>
@@ -29393,7 +29390,7 @@
         <v>644</v>
       </c>
       <c r="B231" t="s" s="2">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C231" t="s" s="2">
         <v>45</v>
@@ -29924,7 +29921,7 @@
         <v>291</v>
       </c>
       <c r="Y235" t="s" s="2">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="Z235" t="s" s="2">
         <v>45</v>
@@ -30354,7 +30351,7 @@
         <v>214</v>
       </c>
       <c r="K239" t="s" s="2">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="L239" t="s" s="2">
         <v>216</v>
@@ -30394,7 +30391,7 @@
         <v>291</v>
       </c>
       <c r="Y239" t="s" s="2">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="Z239" t="s" s="2">
         <v>45</v>
@@ -30447,7 +30444,7 @@
     </row>
     <row r="240" hidden="true">
       <c r="A240" t="s" s="2">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B240" s="2"/>
       <c r="C240" t="s" s="2">
@@ -30562,7 +30559,7 @@
     </row>
     <row r="241" hidden="true">
       <c r="A241" t="s" s="2">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B241" s="2"/>
       <c r="C241" t="s" s="2">
@@ -30679,7 +30676,7 @@
     </row>
     <row r="242" hidden="true">
       <c r="A242" t="s" s="2">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B242" s="2"/>
       <c r="C242" t="s" s="2">
@@ -30798,7 +30795,7 @@
     </row>
     <row r="243" hidden="true">
       <c r="A243" t="s" s="2">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B243" s="2"/>
       <c r="C243" t="s" s="2">
@@ -30915,7 +30912,7 @@
     </row>
     <row r="244" hidden="true">
       <c r="A244" t="s" s="2">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B244" s="2"/>
       <c r="C244" t="s" s="2">
@@ -30955,7 +30952,7 @@
       </c>
       <c r="P244" s="2"/>
       <c r="Q244" t="s" s="2">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="R244" t="s" s="2">
         <v>45</v>
@@ -31032,7 +31029,7 @@
     </row>
     <row r="245" hidden="true">
       <c r="A245" t="s" s="2">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B245" s="2"/>
       <c r="C245" t="s" s="2">
@@ -31149,7 +31146,7 @@
     </row>
     <row r="246" hidden="true">
       <c r="A246" t="s" s="2">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B246" s="2"/>
       <c r="C246" t="s" s="2">
@@ -31296,7 +31293,7 @@
         <v>214</v>
       </c>
       <c r="K247" t="s" s="2">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="L247" t="s" s="2">
         <v>216</v>
@@ -31389,7 +31386,7 @@
     </row>
     <row r="248" hidden="true">
       <c r="A248" t="s" s="2">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B248" s="2"/>
       <c r="C248" t="s" s="2">
@@ -31504,7 +31501,7 @@
     </row>
     <row r="249" hidden="true">
       <c r="A249" t="s" s="2">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B249" s="2"/>
       <c r="C249" t="s" s="2">
@@ -31619,7 +31616,7 @@
     </row>
     <row r="250" hidden="true">
       <c r="A250" t="s" s="2">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B250" t="s" s="2">
         <v>304</v>
@@ -31736,7 +31733,7 @@
     </row>
     <row r="251" hidden="true">
       <c r="A251" t="s" s="2">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B251" s="2"/>
       <c r="C251" t="s" s="2">
@@ -31851,7 +31848,7 @@
     </row>
     <row r="252" hidden="true">
       <c r="A252" t="s" s="2">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B252" s="2"/>
       <c r="C252" t="s" s="2">
@@ -31966,7 +31963,7 @@
     </row>
     <row r="253" hidden="true">
       <c r="A253" t="s" s="2">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B253" t="s" s="2">
         <v>310</v>
@@ -32083,7 +32080,7 @@
     </row>
     <row r="254" hidden="true">
       <c r="A254" t="s" s="2">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B254" s="2"/>
       <c r="C254" t="s" s="2">
@@ -32198,7 +32195,7 @@
     </row>
     <row r="255" hidden="true">
       <c r="A255" t="s" s="2">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B255" s="2"/>
       <c r="C255" t="s" s="2">
@@ -32315,7 +32312,7 @@
     </row>
     <row r="256" hidden="true">
       <c r="A256" t="s" s="2">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B256" s="2"/>
       <c r="C256" t="s" s="2">
@@ -32432,7 +32429,7 @@
     </row>
     <row r="257" hidden="true">
       <c r="A257" t="s" s="2">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B257" t="s" s="2">
         <v>320</v>
@@ -32549,7 +32546,7 @@
     </row>
     <row r="258" hidden="true">
       <c r="A258" t="s" s="2">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B258" t="s" s="2">
         <v>323</v>
@@ -32666,7 +32663,7 @@
     </row>
     <row r="259" hidden="true">
       <c r="A259" t="s" s="2">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B259" s="2"/>
       <c r="C259" t="s" s="2">
@@ -32781,7 +32778,7 @@
     </row>
     <row r="260" hidden="true">
       <c r="A260" t="s" s="2">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B260" s="2"/>
       <c r="C260" t="s" s="2">
@@ -32898,7 +32895,7 @@
     </row>
     <row r="261" hidden="true">
       <c r="A261" t="s" s="2">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B261" s="2"/>
       <c r="C261" t="s" s="2">
@@ -33015,7 +33012,7 @@
     </row>
     <row r="262" hidden="true">
       <c r="A262" t="s" s="2">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B262" t="s" s="2">
         <v>326</v>
@@ -33132,7 +33129,7 @@
     </row>
     <row r="263" hidden="true">
       <c r="A263" t="s" s="2">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B263" s="2"/>
       <c r="C263" t="s" s="2">
@@ -33249,7 +33246,7 @@
     </row>
     <row r="264" hidden="true">
       <c r="A264" t="s" s="2">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B264" s="2"/>
       <c r="C264" t="s" s="2">
@@ -33364,7 +33361,7 @@
     </row>
     <row r="265" hidden="true">
       <c r="A265" t="s" s="2">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B265" s="2"/>
       <c r="C265" t="s" s="2">
@@ -33483,7 +33480,7 @@
     </row>
     <row r="266" hidden="true">
       <c r="A266" t="s" s="2">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B266" s="2"/>
       <c r="C266" t="s" s="2">
@@ -33600,7 +33597,7 @@
     </row>
     <row r="267" hidden="true">
       <c r="A267" t="s" s="2">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B267" s="2"/>
       <c r="C267" t="s" s="2">
@@ -33640,7 +33637,7 @@
       </c>
       <c r="P267" s="2"/>
       <c r="Q267" t="s" s="2">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="R267" t="s" s="2">
         <v>45</v>
@@ -33717,7 +33714,7 @@
     </row>
     <row r="268" hidden="true">
       <c r="A268" t="s" s="2">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B268" s="2"/>
       <c r="C268" t="s" s="2">
@@ -33757,7 +33754,7 @@
       </c>
       <c r="P268" s="2"/>
       <c r="Q268" t="s" s="2">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="R268" t="s" s="2">
         <v>45</v>
@@ -33834,7 +33831,7 @@
     </row>
     <row r="269" hidden="true">
       <c r="A269" t="s" s="2">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B269" s="2"/>
       <c r="C269" t="s" s="2">
@@ -33953,7 +33950,7 @@
     </row>
     <row r="270" hidden="true">
       <c r="A270" t="s" s="2">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B270" s="2"/>
       <c r="C270" t="s" s="2">
@@ -34072,7 +34069,7 @@
     </row>
     <row r="271" hidden="true">
       <c r="A271" t="s" s="2">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B271" t="s" s="2">
         <v>386</v>
@@ -34137,10 +34134,10 @@
         <v>136</v>
       </c>
       <c r="X271" t="s" s="2">
+        <v>700</v>
+      </c>
+      <c r="Y271" t="s" s="2">
         <v>701</v>
-      </c>
-      <c r="Y271" t="s" s="2">
-        <v>702</v>
       </c>
       <c r="Z271" t="s" s="2">
         <v>45</v>
@@ -34193,7 +34190,7 @@
     </row>
     <row r="272" hidden="true">
       <c r="A272" t="s" s="2">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B272" s="2"/>
       <c r="C272" t="s" s="2">
@@ -34308,7 +34305,7 @@
     </row>
     <row r="273" hidden="true">
       <c r="A273" t="s" s="2">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B273" s="2"/>
       <c r="C273" t="s" s="2">
@@ -34425,7 +34422,7 @@
     </row>
     <row r="274" hidden="true">
       <c r="A274" t="s" s="2">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B274" s="2"/>
       <c r="C274" t="s" s="2">
@@ -34544,7 +34541,7 @@
     </row>
     <row r="275" hidden="true">
       <c r="A275" t="s" s="2">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B275" s="2"/>
       <c r="C275" t="s" s="2">
@@ -34665,7 +34662,7 @@
     </row>
     <row r="276" hidden="true">
       <c r="A276" t="s" s="2">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B276" s="2"/>
       <c r="C276" t="s" s="2">
@@ -34782,7 +34779,7 @@
     </row>
     <row r="277" hidden="true">
       <c r="A277" t="s" s="2">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B277" s="2"/>
       <c r="C277" t="s" s="2">
@@ -34899,7 +34896,7 @@
     </row>
     <row r="278" hidden="true">
       <c r="A278" t="s" s="2">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B278" s="2"/>
       <c r="C278" t="s" s="2">
@@ -34925,7 +34922,7 @@
         <v>75</v>
       </c>
       <c r="K278" t="s" s="2">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="L278" t="s" s="2">
         <v>438</v>
@@ -34941,7 +34938,7 @@
       </c>
       <c r="P278" s="2"/>
       <c r="Q278" t="s" s="2">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="R278" t="s" s="2">
         <v>45</v>

</xml_diff>